<commit_message>
Theme 5 data import
</commit_message>
<xml_diff>
--- a/data-governance/CSIEM_Data_Catalogue.xlsx
+++ b/data-governance/CSIEM_Data_Catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60A50DE-8DFB-4550-B359-7E072F84AA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35AB65A-57CB-4E41-81A3-B01FDE6A0CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC9683DB-6EDF-419C-90AE-B9006858D13B}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15540" xr2:uid="{BC9683DB-6EDF-419C-90AE-B9006858D13B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="132">
   <si>
     <t>Group</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Ongoing</t>
+  </si>
+  <si>
+    <t>WWMSP3.1</t>
+  </si>
+  <si>
+    <t>Needs review, but should be removed</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +485,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,6 +535,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,12 +880,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93540D03-D0CE-447B-B6B5-ABD8DB3C1678}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="555" topLeftCell="A10" activePane="bottomLeft"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="450" topLeftCell="A12" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1888,7 +1909,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -1911,7 +1932,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
@@ -1943,71 +1964,68 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="35" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="12">
         <v>18</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="10" t="s">
         <v>129</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="K35" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>116</v>
+        <v>86</v>
+      </c>
+      <c r="H36" s="5">
+        <v>18</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -2021,25 +2039,25 @@
         <v>42</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>116</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
@@ -2053,22 +2071,25 @@
         <v>42</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="I38" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="J38" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -2081,19 +2102,48 @@
       <c r="D39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>127</v>
+      <c r="E39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="5">
         <v>1</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>